<commit_message>
Floc- primary and more navigation drawer design.
</commit_message>
<xml_diff>
--- a/floc_github/Floc_May.xlsx
+++ b/floc_github/Floc_May.xlsx
@@ -33,7 +33,7 @@
     <t>22/5/2017</t>
   </si>
   <si>
-    <t>Added checkbox for don’t show againg feautring screen and home page design</t>
+    <t>Added checkbox for don’t show againg feautring screen and home page design, roughly design primary drawer menu</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>